<commit_message>
OPTIMIZACION DE LAS SIGUIENTES FUNCIONALIDADES: GESTIONCAMIONES GESTIONPILOTOS GESTIONUSUARIOS
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Placas</t>
   </si>
@@ -74,72 +74,69 @@
     <t>Renault</t>
   </si>
   <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>Disel</t>
+  </si>
+  <si>
+    <t>15/01/1900</t>
+  </si>
+  <si>
+    <t>Batería</t>
+  </si>
+  <si>
+    <t>1 semana</t>
+  </si>
+  <si>
+    <t>Ninguno</t>
+  </si>
+  <si>
+    <t>Costo Total Combustible</t>
+  </si>
+  <si>
+    <t>YZA567</t>
+  </si>
+  <si>
+    <t>X9</t>
+  </si>
+  <si>
+    <t>DAF</t>
+  </si>
+  <si>
     <t>En viaje</t>
   </si>
   <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>17/01/1900</t>
+  </si>
+  <si>
+    <t>Transmisión</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>BCD890</t>
+  </si>
+  <si>
+    <t>X10</t>
+  </si>
+  <si>
+    <t>Iveco</t>
+  </si>
+  <si>
     <t>Diésel</t>
   </si>
   <si>
-    <t>17/10/2020</t>
-  </si>
-  <si>
-    <t>Batería</t>
-  </si>
-  <si>
-    <t>4 días</t>
-  </si>
-  <si>
-    <t>18/09/2024</t>
-  </si>
-  <si>
-    <t>Costo Total Combustible</t>
-  </si>
-  <si>
-    <t>YZA567</t>
-  </si>
-  <si>
-    <t>X9</t>
-  </si>
-  <si>
-    <t>DAF</t>
-  </si>
-  <si>
-    <t>Gasolina</t>
-  </si>
-  <si>
-    <t>18/10/2020</t>
-  </si>
-  <si>
-    <t>Transmisión</t>
-  </si>
-  <si>
-    <t>3 días</t>
-  </si>
-  <si>
-    <t>18/12/2023</t>
-  </si>
-  <si>
-    <t>BCD890</t>
-  </si>
-  <si>
-    <t>X10</t>
-  </si>
-  <si>
-    <t>Iveco</t>
-  </si>
-  <si>
     <t>19/10/2020</t>
   </si>
   <si>
     <t>Suspensión</t>
   </si>
   <si>
-    <t>2 días</t>
-  </si>
-  <si>
-    <t>13/09/2024</t>
-  </si>
-  <si>
     <t>EFG123</t>
   </si>
   <si>
@@ -149,21 +146,12 @@
     <t>MEME</t>
   </si>
   <si>
-    <t>Disel</t>
-  </si>
-  <si>
     <t>12/07/1905</t>
   </si>
   <si>
     <t>Radiador</t>
   </si>
   <si>
-    <t>1 días</t>
-  </si>
-  <si>
-    <t>20/12/2023</t>
-  </si>
-  <si>
     <t>HIJ456</t>
   </si>
   <si>
@@ -179,12 +167,6 @@
     <t>Sistema de frenos</t>
   </si>
   <si>
-    <t>0 días</t>
-  </si>
-  <si>
-    <t>21/12/2023</t>
-  </si>
-  <si>
     <t>KLM789</t>
   </si>
   <si>
@@ -203,9 +185,6 @@
     <t>Dirección</t>
   </si>
   <si>
-    <t>22/12/2023</t>
-  </si>
-  <si>
     <t>NOP012</t>
   </si>
   <si>
@@ -221,31 +200,10 @@
     <t>Marcos</t>
   </si>
   <si>
-    <t>10 días</t>
-  </si>
-  <si>
-    <t>En mantenimiento</t>
-  </si>
-  <si>
     <t>24/10/2020</t>
   </si>
   <si>
     <t>Revisión completa</t>
-  </si>
-  <si>
-    <t>24/12/2023</t>
-  </si>
-  <si>
-    <t>1R</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>16/07/1905</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -290,7 +248,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -381,10 +339,10 @@
         <v>0.0</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>27.55</v>
+        <v>0.0</v>
       </c>
       <c r="K2" t="n" s="0">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="L2" t="n" s="0">
         <v>0.0</v>
@@ -402,7 +360,7 @@
         <v>25</v>
       </c>
       <c r="Q2" t="n" s="0">
-        <v>2.842170943040401E-14</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -416,10 +374,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>22000.0</v>
@@ -428,7 +386,7 @@
         <v>1600.0</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" t="n" s="0">
         <v>0.0</v>
@@ -446,13 +404,13 @@
         <v>0.0</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="n" s="0">
         <v>0.0</v>
@@ -469,10 +427,10 @@
         <v>37</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>28000.0</v>
@@ -481,7 +439,7 @@
         <v>1800.0</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" t="n" s="0">
         <v>0.0</v>
@@ -499,13 +457,13 @@
         <v>0.0</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="P4" t="s" s="0">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="n" s="0">
         <v>0.0</v>
@@ -513,19 +471,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="C5" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>44</v>
-      </c>
       <c r="D5" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F5" t="n" s="0">
         <v>15000.0</v>
@@ -534,7 +492,7 @@
         <v>1900.0</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>0.0</v>
@@ -552,13 +510,13 @@
         <v>0.0</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="n" s="0">
         <v>0.0</v>
@@ -566,19 +524,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" t="n" s="0">
         <v>40000.0</v>
@@ -587,7 +545,7 @@
         <v>2100.0</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>0.0</v>
@@ -605,13 +563,13 @@
         <v>0.0</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s" s="0">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="P6" t="s" s="0">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="Q6" t="n" s="0">
         <v>0.0</v>
@@ -619,19 +577,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F7" t="n" s="0">
         <v>18000.0</v>
@@ -640,7 +598,7 @@
         <v>2000.0</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I7" t="n" s="0">
         <v>0.0</v>
@@ -658,13 +616,13 @@
         <v>0.0</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="P7" t="s" s="0">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="Q7" t="n" s="0">
         <v>0.0</v>
@@ -672,19 +630,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" t="n" s="0">
         <v>32000.0</v>
@@ -693,7 +651,7 @@
         <v>1600.0</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I8" t="n" s="0">
         <v>0.0</v>
@@ -711,13 +669,13 @@
         <v>0.0</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="O8" t="s" s="0">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="P8" t="s" s="0">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="Q8" t="n" s="0">
         <v>0.0</v>
@@ -725,19 +683,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F9" t="n" s="0">
         <v>25000.0</v>
@@ -746,7 +704,7 @@
         <v>1800.0</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I9" t="n" s="0">
         <v>0.0</v>
@@ -764,68 +722,15 @@
         <v>0.0</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="O9" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P9" t="s" s="0">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="Q9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>74</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="F10" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="G10" t="n" s="0">
-        <v>1000.0</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="I10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N10" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="O10" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="P10" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="Q10" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IMPLEMENTACION DE GUARDADO DE LA ENTRADA Y SALIDA DEL USUARIO
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -119,6 +119,9 @@
     <t/>
   </si>
   <si>
+    <t>10/10/2024</t>
+  </si>
+  <si>
     <t>BCD890</t>
   </si>
   <si>
@@ -176,10 +179,7 @@
     <t>Freightliner</t>
   </si>
   <si>
-    <t>Disponible</t>
-  </si>
-  <si>
-    <t>22/10/2020</t>
+    <t>21/01/1900</t>
   </si>
   <si>
     <t>Dirección</t>
@@ -398,7 +398,7 @@
         <v>0.0</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="M3" t="n" s="0">
         <v>0.0</v>
@@ -410,27 +410,27 @@
         <v>34</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="n" s="0">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>28000.0</v>
@@ -439,7 +439,7 @@
         <v>1800.0</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" t="n" s="0">
         <v>0.0</v>
@@ -457,7 +457,7 @@
         <v>0.0</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O4" t="s" s="0">
         <v>34</v>
@@ -471,13 +471,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>30</v>
@@ -492,7 +492,7 @@
         <v>1900.0</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>0.0</v>
@@ -510,7 +510,7 @@
         <v>0.0</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O5" t="s" s="0">
         <v>34</v>
@@ -524,13 +524,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>30</v>
@@ -545,7 +545,7 @@
         <v>2100.0</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>0.0</v>
@@ -563,7 +563,7 @@
         <v>0.0</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O6" t="s" s="0">
         <v>34</v>
@@ -577,19 +577,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F7" t="n" s="0">
         <v>18000.0</v>
@@ -683,19 +683,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>30</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" t="n" s="0">
         <v>25000.0</v>

</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑO NO.6
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Placas</t>
   </si>
@@ -68,6 +68,9 @@
     <t>Costo Total Combustible</t>
   </si>
   <si>
+    <t>Activo</t>
+  </si>
+  <si>
     <t>VWX234</t>
   </si>
   <si>
@@ -83,7 +86,7 @@
     <t>Disel</t>
   </si>
   <si>
-    <t>13/01/1900</t>
+    <t>23/10/2014</t>
   </si>
   <si>
     <t>Batería</t>
@@ -95,6 +98,48 @@
     <t>12/10/2024</t>
   </si>
   <si>
+    <t>HIJ456</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>VolvoE</t>
+  </si>
+  <si>
+    <t>En viaje</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>27/10/2018</t>
+  </si>
+  <si>
+    <t>Sistema de frenos</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Ninguno</t>
+  </si>
+  <si>
+    <t>EFG123</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>MEME</t>
+  </si>
+  <si>
+    <t>26/10/2017</t>
+  </si>
+  <si>
+    <t>Radiador</t>
+  </si>
+  <si>
     <t>YZA567</t>
   </si>
   <si>
@@ -104,21 +149,12 @@
     <t>DAF</t>
   </si>
   <si>
-    <t>En viaje</t>
-  </si>
-  <si>
-    <t>Gasolina</t>
-  </si>
-  <si>
-    <t>2005</t>
+    <t>24/10/2015</t>
   </si>
   <si>
     <t>Transmisión</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>11/10/2024</t>
   </si>
   <si>
@@ -128,73 +164,10 @@
     <t>X10</t>
   </si>
   <si>
-    <t>Iveco</t>
-  </si>
-  <si>
-    <t>27/06/1905</t>
+    <t>25/10/2016</t>
   </si>
   <si>
     <t>Suspensión</t>
-  </si>
-  <si>
-    <t>Ninguno</t>
-  </si>
-  <si>
-    <t>EFG123</t>
-  </si>
-  <si>
-    <t>X11</t>
-  </si>
-  <si>
-    <t>MEME</t>
-  </si>
-  <si>
-    <t>12/07/1905</t>
-  </si>
-  <si>
-    <t>Radiador</t>
-  </si>
-  <si>
-    <t>HIJ456</t>
-  </si>
-  <si>
-    <t>X12</t>
-  </si>
-  <si>
-    <t>VolvoE</t>
-  </si>
-  <si>
-    <t>20/01/1900</t>
-  </si>
-  <si>
-    <t>Sistema de frenos</t>
-  </si>
-  <si>
-    <t>KLM789</t>
-  </si>
-  <si>
-    <t>X13</t>
-  </si>
-  <si>
-    <t>Freightliner</t>
-  </si>
-  <si>
-    <t>Dirección</t>
-  </si>
-  <si>
-    <t>NOP012</t>
-  </si>
-  <si>
-    <t>X14</t>
-  </si>
-  <si>
-    <t>Kenworth</t>
-  </si>
-  <si>
-    <t>23/10/2020</t>
-  </si>
-  <si>
-    <t>Marcos</t>
   </si>
 </sst>
 </file>
@@ -239,7 +212,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -300,22 +273,25 @@
       <c r="R1" t="s" s="0">
         <v>17</v>
       </c>
+      <c r="S1" t="s" s="0">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>35000.0</v>
@@ -324,7 +300,7 @@
         <v>1700.0</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" t="n" s="0">
         <v>0.0</v>
@@ -342,45 +318,48 @@
         <v>0.0</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="n" s="0">
         <v>168.0</v>
       </c>
       <c r="R2" t="n" s="0">
         <v>0.0</v>
+      </c>
+      <c r="S2" t="b" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>22000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>1600.0</v>
+        <v>2100.0</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I3" t="n" s="0">
         <v>0.0</v>
@@ -392,81 +371,87 @@
         <v>0.0</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="M3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q3" t="n" s="0">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="R3" t="n" s="0">
         <v>0.0</v>
+      </c>
+      <c r="S3" t="b" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>15000.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>1900.0</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="I4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>28000.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>1800.0</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="I4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N4" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="P4" t="s" s="0">
-        <v>41</v>
-      </c>
       <c r="Q4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="R4" t="n" s="0">
         <v>0.0</v>
+      </c>
+      <c r="S4" t="b" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -480,16 +465,16 @@
         <v>44</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>15000.0</v>
+        <v>22000.0</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>1900.0</v>
+        <v>1600.0</v>
       </c>
       <c r="H5" t="s" s="0">
         <v>45</v>
@@ -504,7 +489,7 @@
         <v>0.0</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="M5" t="n" s="0">
         <v>0.0</v>
@@ -513,39 +498,42 @@
         <v>46</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="Q5" t="n" s="0">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="R5" t="n" s="0">
         <v>0.0</v>
+      </c>
+      <c r="S5" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>40000.0</v>
+        <v>28000.0</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>2100.0</v>
+        <v>1800.0</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>50</v>
@@ -569,10 +557,10 @@
         <v>51</v>
       </c>
       <c r="O6" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P6" t="s" s="0">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q6" t="n" s="0">
         <v>0.0</v>
@@ -580,117 +568,8 @@
       <c r="R6" t="n" s="0">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F7" t="n" s="0">
-        <v>18000.0</v>
-      </c>
-      <c r="G7" t="n" s="0">
-        <v>2000.0</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="I7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N7" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="O7" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="P7" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="Q7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>32000.0</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>1600.0</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="I8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N8" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="P8" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="Q8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R8" t="n" s="0">
-        <v>0.0</v>
+      <c r="S6" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OPTIMIZACION DE PROCESOS Y DISEÑO NO.8
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>Placas</t>
   </si>
@@ -71,6 +71,114 @@
     <t>Activo</t>
   </si>
   <si>
+    <t>PQR345</t>
+  </si>
+  <si>
+    <t>X15</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>FUNCIONAL</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>29/10/2017</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>DEF890</t>
+  </si>
+  <si>
+    <t>X20</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>28/10/2016</t>
+  </si>
+  <si>
+    <t>VWX567</t>
+  </si>
+  <si>
+    <t>X17</t>
+  </si>
+  <si>
+    <t>Iveco</t>
+  </si>
+  <si>
+    <t>Diésel</t>
+  </si>
+  <si>
+    <t>26/10/2018</t>
+  </si>
+  <si>
+    <t>DEF456</t>
+  </si>
+  <si>
+    <t>X9</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>22/10/2016</t>
+  </si>
+  <si>
+    <t>XYZ678</t>
+  </si>
+  <si>
+    <t>X18</t>
+  </si>
+  <si>
+    <t>Hino</t>
+  </si>
+  <si>
+    <t>27/10/2015</t>
+  </si>
+  <si>
+    <t>GHI789</t>
+  </si>
+  <si>
+    <t>X10</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>21/10/2015</t>
+  </si>
+  <si>
+    <t>GHI012</t>
+  </si>
+  <si>
+    <t>X21</t>
+  </si>
+  <si>
+    <t>Kenworth</t>
+  </si>
+  <si>
+    <t>30/10/2020</t>
+  </si>
+  <si>
+    <t>HIJ456</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>VolvoE</t>
+  </si>
+  <si>
+    <t>27/10/2018</t>
+  </si>
+  <si>
     <t>VWX234</t>
   </si>
   <si>
@@ -80,7 +188,7 @@
     <t>Mynor</t>
   </si>
   <si>
-    <t>Funcional</t>
+    <t>DESCOMPUESTO</t>
   </si>
   <si>
     <t>Disel</t>
@@ -89,40 +197,55 @@
     <t>23/10/2014</t>
   </si>
   <si>
-    <t>Batería</t>
-  </si>
-  <si>
-    <t>1 semana</t>
-  </si>
-  <si>
-    <t>12/10/2024</t>
-  </si>
-  <si>
-    <t>HIJ456</t>
-  </si>
-  <si>
-    <t>X12</t>
-  </si>
-  <si>
-    <t>VolvoE</t>
-  </si>
-  <si>
-    <t>En viaje</t>
-  </si>
-  <si>
-    <t>Gasolina</t>
-  </si>
-  <si>
-    <t>27/10/2018</t>
-  </si>
-  <si>
-    <t>Sistema de frenos</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Ninguno</t>
+    <t>ABC789</t>
+  </si>
+  <si>
+    <t>X19</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>23/10/2017</t>
+  </si>
+  <si>
+    <t>MNO234</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>Scania</t>
+  </si>
+  <si>
+    <t>25/10/2014</t>
+  </si>
+  <si>
+    <t>JKL123</t>
+  </si>
+  <si>
+    <t>X13</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>28/10/2020</t>
+  </si>
+  <si>
+    <t>STU456</t>
+  </si>
+  <si>
+    <t>X16</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Eléctrico</t>
+  </si>
+  <si>
+    <t>24/10/2019</t>
   </si>
   <si>
     <t>EFG123</t>
@@ -135,39 +258,6 @@
   </si>
   <si>
     <t>26/10/2017</t>
-  </si>
-  <si>
-    <t>Radiador</t>
-  </si>
-  <si>
-    <t>YZA567</t>
-  </si>
-  <si>
-    <t>X9</t>
-  </si>
-  <si>
-    <t>DAF</t>
-  </si>
-  <si>
-    <t>24/10/2015</t>
-  </si>
-  <si>
-    <t>Transmisión</t>
-  </si>
-  <si>
-    <t>11/10/2024</t>
-  </si>
-  <si>
-    <t>BCD890</t>
-  </si>
-  <si>
-    <t>X10</t>
-  </si>
-  <si>
-    <t>25/10/2016</t>
-  </si>
-  <si>
-    <t>Suspensión</t>
   </si>
 </sst>
 </file>
@@ -212,7 +302,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -294,10 +384,10 @@
         <v>23</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>35000.0</v>
+        <v>47000.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>1700.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>24</v>
@@ -306,13 +396,13 @@
         <v>0.0</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="K2" t="n" s="0">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="L2" t="n" s="0">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="M2" t="n" s="0">
         <v>0.0</v>
@@ -321,46 +411,46 @@
         <v>25</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="n" s="0">
-        <v>168.0</v>
+        <v>0.0</v>
       </c>
       <c r="R2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="S2" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="D3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>31000.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>2000.0</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>40000.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>2100.0</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>33</v>
-      </c>
       <c r="I3" t="n" s="0">
         <v>0.0</v>
       </c>
@@ -377,13 +467,13 @@
         <v>0.0</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="n" s="0">
         <v>0.0</v>
@@ -392,33 +482,33 @@
         <v>0.0</v>
       </c>
       <c r="S3" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>15000.0</v>
+        <v>38000.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>1900.0</v>
+        <v>2100.0</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I4" t="n" s="0">
         <v>0.0</v>
@@ -436,13 +526,13 @@
         <v>0.0</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s" s="0">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="n" s="0">
         <v>0.0</v>
@@ -451,33 +541,33 @@
         <v>0.0</v>
       </c>
       <c r="S4" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>22000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>1600.0</v>
+        <v>2000.0</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>0.0</v>
@@ -489,22 +579,22 @@
         <v>0.0</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="M5" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="n" s="0">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="R5" t="n" s="0">
         <v>0.0</v>
@@ -515,60 +605,591 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F6" t="n" s="0">
+        <v>34000.0</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>2200.0</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S6" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F7" t="n" s="0">
         <v>28000.0</v>
       </c>
-      <c r="G6" t="n" s="0">
+      <c r="G7" t="n" s="0">
+        <v>1600.0</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S7" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>45000.0</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>2500.0</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="I8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S8" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>40000.0</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>2100.0</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S9" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>35000.0</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>1700.0</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="I10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S10" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>27000.0</v>
+      </c>
+      <c r="G11" t="n" s="0">
+        <v>2300.0</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="I11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S11" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>32000.0</v>
+      </c>
+      <c r="G12" t="n" s="0">
+        <v>1900.0</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="I12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S12" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>45000.0</v>
+      </c>
+      <c r="G13" t="n" s="0">
+        <v>2200.0</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="I13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S13" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>26000.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
         <v>1800.0</v>
       </c>
-      <c r="H6" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="I6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="P6" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="Q6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="S6" t="b" s="0">
+      <c r="H14" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="I14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N14" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O14" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P14" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S14" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F15" t="n" s="0">
+        <v>15000.0</v>
+      </c>
+      <c r="G15" t="n" s="0">
+        <v>1900.0</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="I15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N15" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O15" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P15" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S15" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑOS Y PROCESOS NO.11
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="173">
   <si>
     <t>Placas</t>
   </si>
@@ -71,6 +71,45 @@
     <t>Activo</t>
   </si>
   <si>
+    <t>ABC345</t>
+  </si>
+  <si>
+    <t>X24</t>
+  </si>
+  <si>
+    <t>Iveco</t>
+  </si>
+  <si>
+    <t>INACTIVO</t>
+  </si>
+  <si>
+    <t>Diésel</t>
+  </si>
+  <si>
+    <t>27/10/2015</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>DEF234</t>
+  </si>
+  <si>
+    <t>U2100</t>
+  </si>
+  <si>
+    <t>Isuzu</t>
+  </si>
+  <si>
+    <t>30/09/2017</t>
+  </si>
+  <si>
+    <t>31/12/1899</t>
+  </si>
+  <si>
     <t>PQR345</t>
   </si>
   <si>
@@ -80,37 +119,58 @@
     <t>MAN</t>
   </si>
   <si>
-    <t>INACTIVO</t>
-  </si>
-  <si>
     <t>Gasolina</t>
   </si>
   <si>
     <t>29/10/2017</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>0.0</t>
+    <t>JKL012</t>
+  </si>
+  <si>
+    <t>D400</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>30/10/2020</t>
+  </si>
+  <si>
+    <t>EFG456</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>Kenworth</t>
+  </si>
+  <si>
+    <t>21/10/2015</t>
   </si>
   <si>
     <t>EFG123</t>
   </si>
   <si>
-    <t>X11</t>
-  </si>
-  <si>
     <t>Scania</t>
   </si>
   <si>
+    <t>26/10/2017</t>
+  </si>
+  <si>
+    <t>DEF456</t>
+  </si>
+  <si>
+    <t>B200</t>
+  </si>
+  <si>
+    <t>Hino</t>
+  </si>
+  <si>
     <t>FUNCIONAL</t>
   </si>
   <si>
-    <t>Diésel</t>
-  </si>
-  <si>
-    <t>26/10/2017</t>
+    <t>22/06/2018</t>
   </si>
   <si>
     <t>DEF890</t>
@@ -131,9 +191,6 @@
     <t>X17</t>
   </si>
   <si>
-    <t>Iveco</t>
-  </si>
-  <si>
     <t>26/10/2018</t>
   </si>
   <si>
@@ -152,379 +209,325 @@
     <t>24/10/2019</t>
   </si>
   <si>
-    <t>DEF456</t>
-  </si>
-  <si>
-    <t>X9</t>
+    <t>GHI012</t>
+  </si>
+  <si>
+    <t>MEME</t>
+  </si>
+  <si>
+    <t>Nissa</t>
+  </si>
+  <si>
+    <t>Disel</t>
+  </si>
+  <si>
+    <t>ABC789</t>
+  </si>
+  <si>
+    <t>X19</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>23/10/2017</t>
+  </si>
+  <si>
+    <t>HIJ456</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>27/10/2018</t>
+  </si>
+  <si>
+    <t>XYZ678</t>
+  </si>
+  <si>
+    <t>X18</t>
+  </si>
+  <si>
+    <t>MNO234</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>25/10/2014</t>
+  </si>
+  <si>
+    <t>STU789</t>
+  </si>
+  <si>
+    <t>22/10/2016</t>
+  </si>
+  <si>
+    <t>HIJ789</t>
+  </si>
+  <si>
+    <t>23/10/2014</t>
+  </si>
+  <si>
+    <t>VWX123</t>
+  </si>
+  <si>
+    <t>X21</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>DEF123</t>
+  </si>
+  <si>
+    <t>X22</t>
   </si>
   <si>
     <t>Toyota</t>
   </si>
   <si>
-    <t>22/10/2016</t>
+    <t>GHI123</t>
+  </si>
+  <si>
+    <t>X23</t>
+  </si>
+  <si>
+    <t>XYZ123</t>
+  </si>
+  <si>
+    <t>A100</t>
+  </si>
+  <si>
+    <t>12/04/2019</t>
   </si>
   <si>
     <t>GHI789</t>
   </si>
   <si>
-    <t>X10</t>
-  </si>
-  <si>
-    <t>Ford</t>
-  </si>
-  <si>
-    <t>21/10/2015</t>
-  </si>
-  <si>
-    <t>GHI012</t>
-  </si>
-  <si>
-    <t>X21</t>
-  </si>
-  <si>
-    <t>Kenworth</t>
-  </si>
-  <si>
-    <t>30/10/2020</t>
-  </si>
-  <si>
-    <t>ABC789</t>
-  </si>
-  <si>
-    <t>X19</t>
-  </si>
-  <si>
-    <t>Mercedes</t>
-  </si>
-  <si>
-    <t>23/10/2017</t>
-  </si>
-  <si>
-    <t>HIJ456</t>
-  </si>
-  <si>
-    <t>X12</t>
-  </si>
-  <si>
-    <t>27/10/2018</t>
+    <t>C300</t>
+  </si>
+  <si>
+    <t>Freightliner</t>
+  </si>
+  <si>
+    <t>14/09/2017</t>
+  </si>
+  <si>
+    <t>MNO345</t>
+  </si>
+  <si>
+    <t>E500</t>
+  </si>
+  <si>
+    <t>28/02/2016</t>
+  </si>
+  <si>
+    <t>PQR678</t>
+  </si>
+  <si>
+    <t>F600</t>
+  </si>
+  <si>
+    <t>Mack</t>
+  </si>
+  <si>
+    <t>15/11/2018</t>
+  </si>
+  <si>
+    <t>STU901</t>
+  </si>
+  <si>
+    <t>G700</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>20/03/2019</t>
+  </si>
+  <si>
+    <t>VWX234</t>
+  </si>
+  <si>
+    <t>H800</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>05/08/2016</t>
+  </si>
+  <si>
+    <t>12/10/2024</t>
+  </si>
+  <si>
+    <t>YZA567</t>
+  </si>
+  <si>
+    <t>I900</t>
+  </si>
+  <si>
+    <t>15/09/2017</t>
+  </si>
+  <si>
+    <t>11/10/2024</t>
+  </si>
+  <si>
+    <t>BCD890</t>
+  </si>
+  <si>
+    <t>J1000</t>
+  </si>
+  <si>
+    <t>22/01/2020</t>
+  </si>
+  <si>
+    <t>EFG234</t>
+  </si>
+  <si>
+    <t>K1100</t>
+  </si>
+  <si>
+    <t>12/06/2019</t>
+  </si>
+  <si>
+    <t>GHI567</t>
+  </si>
+  <si>
+    <t>L1200</t>
+  </si>
+  <si>
+    <t>30/04/2018</t>
+  </si>
+  <si>
+    <t>JKL890</t>
+  </si>
+  <si>
+    <t>M1300</t>
+  </si>
+  <si>
+    <t>10/02/2021</t>
+  </si>
+  <si>
+    <t>NOP123</t>
+  </si>
+  <si>
+    <t>N1400</t>
+  </si>
+  <si>
+    <t>01/07/2016</t>
+  </si>
+  <si>
+    <t>QRS456</t>
+  </si>
+  <si>
+    <t>O1500</t>
+  </si>
+  <si>
+    <t>15/11/2019</t>
+  </si>
+  <si>
+    <t>P1600</t>
+  </si>
+  <si>
+    <t>20/05/2017</t>
+  </si>
+  <si>
+    <t>TUV012</t>
+  </si>
+  <si>
+    <t>1700.0</t>
+  </si>
+  <si>
+    <t>10/03/2018</t>
+  </si>
+  <si>
+    <t>VWX345</t>
+  </si>
+  <si>
+    <t>R1800</t>
+  </si>
+  <si>
+    <t>01/01/2016</t>
+  </si>
+  <si>
+    <t>S1900</t>
+  </si>
+  <si>
+    <t>22/04/2020</t>
+  </si>
+  <si>
+    <t>ABC901</t>
+  </si>
+  <si>
+    <t>T2000</t>
+  </si>
+  <si>
+    <t>15/08/2019</t>
+  </si>
+  <si>
+    <t>V2200</t>
+  </si>
+  <si>
+    <t>12/02/2018</t>
+  </si>
+  <si>
+    <t>XYZ234</t>
+  </si>
+  <si>
+    <t>X250</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>14/03/2020</t>
+  </si>
+  <si>
+    <t>DEF567</t>
+  </si>
+  <si>
+    <t>Y260</t>
+  </si>
+  <si>
+    <t>Fuso</t>
+  </si>
+  <si>
+    <t>22/05/2019</t>
+  </si>
+  <si>
+    <t>GHI890</t>
+  </si>
+  <si>
+    <t>Z270</t>
+  </si>
+  <si>
+    <t>10/07/2018</t>
   </si>
   <si>
     <t>JKL123</t>
   </si>
   <si>
-    <t>X13</t>
-  </si>
-  <si>
-    <t>Nissan</t>
-  </si>
-  <si>
-    <t>28/10/2020</t>
-  </si>
-  <si>
-    <t>XYZ678</t>
-  </si>
-  <si>
-    <t>X18</t>
-  </si>
-  <si>
-    <t>Hino</t>
-  </si>
-  <si>
-    <t>27/10/2015</t>
-  </si>
-  <si>
-    <t>MNO234</t>
-  </si>
-  <si>
-    <t>X14</t>
-  </si>
-  <si>
-    <t>25/10/2014</t>
+    <t>A280</t>
+  </si>
+  <si>
+    <t>18/10/2021</t>
+  </si>
+  <si>
+    <t>MNO456</t>
+  </si>
+  <si>
+    <t>B290</t>
+  </si>
+  <si>
+    <t>DAF</t>
+  </si>
+  <si>
+    <t>22/08/2020</t>
   </si>
   <si>
     <t>PQR789</t>
-  </si>
-  <si>
-    <t>STU789</t>
-  </si>
-  <si>
-    <t>EFG456</t>
-  </si>
-  <si>
-    <t>HIJ789</t>
-  </si>
-  <si>
-    <t>23/10/2014</t>
-  </si>
-  <si>
-    <t>VWX123</t>
-  </si>
-  <si>
-    <t>DEF123</t>
-  </si>
-  <si>
-    <t>X22</t>
-  </si>
-  <si>
-    <t>GHI123</t>
-  </si>
-  <si>
-    <t>X23</t>
-  </si>
-  <si>
-    <t>ABC345</t>
-  </si>
-  <si>
-    <t>X24</t>
-  </si>
-  <si>
-    <t>XYZ123</t>
-  </si>
-  <si>
-    <t>A100</t>
-  </si>
-  <si>
-    <t>Isuzu</t>
-  </si>
-  <si>
-    <t>12/04/2019</t>
-  </si>
-  <si>
-    <t>31/12/1899</t>
-  </si>
-  <si>
-    <t>B200</t>
-  </si>
-  <si>
-    <t>22/06/2018</t>
-  </si>
-  <si>
-    <t>C300</t>
-  </si>
-  <si>
-    <t>Freightliner</t>
-  </si>
-  <si>
-    <t>14/09/2017</t>
-  </si>
-  <si>
-    <t>JKL012</t>
-  </si>
-  <si>
-    <t>D400</t>
-  </si>
-  <si>
-    <t>Mitsubishi</t>
-  </si>
-  <si>
-    <t>MNO345</t>
-  </si>
-  <si>
-    <t>E500</t>
-  </si>
-  <si>
-    <t>28/02/2016</t>
-  </si>
-  <si>
-    <t>PQR678</t>
-  </si>
-  <si>
-    <t>F600</t>
-  </si>
-  <si>
-    <t>Mack</t>
-  </si>
-  <si>
-    <t>15/11/2018</t>
-  </si>
-  <si>
-    <t>STU901</t>
-  </si>
-  <si>
-    <t>G700</t>
-  </si>
-  <si>
-    <t>International</t>
-  </si>
-  <si>
-    <t>20/03/2019</t>
-  </si>
-  <si>
-    <t>VWX234</t>
-  </si>
-  <si>
-    <t>H800</t>
-  </si>
-  <si>
-    <t>05/08/2016</t>
-  </si>
-  <si>
-    <t>YZA567</t>
-  </si>
-  <si>
-    <t>I900</t>
-  </si>
-  <si>
-    <t>15/09/2017</t>
-  </si>
-  <si>
-    <t>BCD890</t>
-  </si>
-  <si>
-    <t>J1000</t>
-  </si>
-  <si>
-    <t>22/01/2020</t>
-  </si>
-  <si>
-    <t>EFG234</t>
-  </si>
-  <si>
-    <t>K1100</t>
-  </si>
-  <si>
-    <t>12/06/2019</t>
-  </si>
-  <si>
-    <t>GHI567</t>
-  </si>
-  <si>
-    <t>L1200</t>
-  </si>
-  <si>
-    <t>30/04/2018</t>
-  </si>
-  <si>
-    <t>JKL890</t>
-  </si>
-  <si>
-    <t>M1300</t>
-  </si>
-  <si>
-    <t>10/02/2021</t>
-  </si>
-  <si>
-    <t>NOP123</t>
-  </si>
-  <si>
-    <t>N1400</t>
-  </si>
-  <si>
-    <t>01/07/2016</t>
-  </si>
-  <si>
-    <t>QRS456</t>
-  </si>
-  <si>
-    <t>O1500</t>
-  </si>
-  <si>
-    <t>15/11/2019</t>
-  </si>
-  <si>
-    <t>P1600</t>
-  </si>
-  <si>
-    <t>20/05/2017</t>
-  </si>
-  <si>
-    <t>TUV012</t>
-  </si>
-  <si>
-    <t>1700.0</t>
-  </si>
-  <si>
-    <t>10/03/2018</t>
-  </si>
-  <si>
-    <t>VWX345</t>
-  </si>
-  <si>
-    <t>R1800</t>
-  </si>
-  <si>
-    <t>01/01/2016</t>
-  </si>
-  <si>
-    <t>S1900</t>
-  </si>
-  <si>
-    <t>22/04/2020</t>
-  </si>
-  <si>
-    <t>ABC901</t>
-  </si>
-  <si>
-    <t>T2000</t>
-  </si>
-  <si>
-    <t>15/08/2019</t>
-  </si>
-  <si>
-    <t>DEF234</t>
-  </si>
-  <si>
-    <t>U2100</t>
-  </si>
-  <si>
-    <t>30/09/2017</t>
-  </si>
-  <si>
-    <t>V2200</t>
-  </si>
-  <si>
-    <t>12/02/2018</t>
-  </si>
-  <si>
-    <t>XYZ234</t>
-  </si>
-  <si>
-    <t>X250</t>
-  </si>
-  <si>
-    <t>Tata</t>
-  </si>
-  <si>
-    <t>14/03/2020</t>
-  </si>
-  <si>
-    <t>DEF567</t>
-  </si>
-  <si>
-    <t>Y260</t>
-  </si>
-  <si>
-    <t>Fuso</t>
-  </si>
-  <si>
-    <t>22/05/2019</t>
-  </si>
-  <si>
-    <t>GHI890</t>
-  </si>
-  <si>
-    <t>Z270</t>
-  </si>
-  <si>
-    <t>10/07/2018</t>
-  </si>
-  <si>
-    <t>A280</t>
-  </si>
-  <si>
-    <t>18/10/2021</t>
-  </si>
-  <si>
-    <t>MNO456</t>
-  </si>
-  <si>
-    <t>B290</t>
-  </si>
-  <si>
-    <t>DAF</t>
-  </si>
-  <si>
-    <t>22/08/2020</t>
   </si>
   <si>
     <t>05/02/2019</t>
@@ -572,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -648,16 +651,16 @@
         <v>21</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>47000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>2400.0</v>
+        <v>2200.0</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>24</v>
@@ -707,44 +710,44 @@
         <v>29</v>
       </c>
       <c r="D3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>41000.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>2200.0</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="I3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="F3" t="n" s="0">
-        <v>15000.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>1900.0</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N3" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s" s="0">
-        <v>25</v>
-      </c>
       <c r="Q3" t="n" s="0">
         <v>0.0</v>
       </c>
@@ -752,30 +755,30 @@
         <v>0.0</v>
       </c>
       <c r="S3" t="b" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>23</v>
-      </c>
       <c r="F4" t="n" s="0">
-        <v>31000.0</v>
+        <v>47000.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>2000.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>36</v>
@@ -811,7 +814,7 @@
         <v>0.0</v>
       </c>
       <c r="S4" t="b" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -825,13 +828,13 @@
         <v>39</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>38000.0</v>
+        <v>29000.0</v>
       </c>
       <c r="G5" t="n" s="0">
         <v>2100.0</v>
@@ -861,7 +864,7 @@
         <v>26</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="Q5" t="n" s="0">
         <v>0.0</v>
@@ -884,19 +887,19 @@
         <v>43</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>28000.0</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>1600.0</v>
+      </c>
+      <c r="H6" t="s" s="0">
         <v>44</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <v>26000.0</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <v>1800.0</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>45</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>0.0</v>
@@ -934,28 +937,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>48</v>
-      </c>
       <c r="D7" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>30000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>2000.0</v>
+        <v>1900.0</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I7" t="n" s="0">
         <v>0.0</v>
@@ -993,52 +996,52 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s" s="0">
+      <c r="D8" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>31000.0</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>1900.0</v>
+      </c>
+      <c r="H8" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="D8" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s" s="0">
+      <c r="I8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>28000.0</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>1600.0</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="I8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P8" t="s" s="0">
-        <v>25</v>
       </c>
       <c r="Q8" t="n" s="0">
         <v>0.0</v>
@@ -1052,28 +1055,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="C9" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="D9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>31000.0</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>2000.0</v>
+      </c>
+      <c r="H9" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F9" t="n" s="0">
-        <v>45000.0</v>
-      </c>
-      <c r="G9" t="n" s="0">
-        <v>2500.0</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>57</v>
       </c>
       <c r="I9" t="n" s="0">
         <v>0.0</v>
@@ -1111,28 +1114,28 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="C10" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>38000.0</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>2100.0</v>
+      </c>
+      <c r="H10" t="s" s="0">
         <v>59</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F10" t="n" s="0">
-        <v>27000.0</v>
-      </c>
-      <c r="G10" t="n" s="0">
-        <v>2300.0</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>61</v>
       </c>
       <c r="I10" t="n" s="0">
         <v>0.0</v>
@@ -1170,25 +1173,25 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="D11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C11" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>23</v>
-      </c>
       <c r="F11" t="n" s="0">
-        <v>40000.0</v>
+        <v>26000.0</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>2100.0</v>
+        <v>1800.0</v>
       </c>
       <c r="H11" t="s" s="0">
         <v>64</v>
@@ -1238,19 +1241,19 @@
         <v>67</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="F12" t="n" s="0">
         <v>45000.0</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>2200.0</v>
+        <v>2500.0</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="I12" t="n" s="0">
         <v>0.0</v>
@@ -1297,16 +1300,16 @@
         <v>71</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>34000.0</v>
+        <v>27000.0</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>2200.0</v>
+        <v>2300.0</v>
       </c>
       <c r="H13" t="s" s="0">
         <v>72</v>
@@ -1353,19 +1356,19 @@
         <v>74</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>32000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="G14" t="n" s="0">
-        <v>1900.0</v>
+        <v>2100.0</v>
       </c>
       <c r="H14" t="s" s="0">
         <v>75</v>
@@ -1409,22 +1412,22 @@
         <v>76</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>47000.0</v>
+        <v>34000.0</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>2400.0</v>
+        <v>2200.0</v>
       </c>
       <c r="H15" t="s" s="0">
         <v>24</v>
@@ -1465,28 +1468,28 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>31000.0</v>
+        <v>32000.0</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>2000.0</v>
+        <v>1900.0</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="I16" t="n" s="0">
         <v>0.0</v>
@@ -1524,28 +1527,28 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>28000.0</v>
+        <v>31000.0</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>1600.0</v>
+        <v>2000.0</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="I17" t="n" s="0">
         <v>0.0</v>
@@ -1583,19 +1586,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F18" t="n" s="0">
         <v>32000.0</v>
@@ -1604,7 +1607,7 @@
         <v>1700.0</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I18" t="n" s="0">
         <v>0.0</v>
@@ -1642,19 +1645,19 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F19" t="n" s="0">
         <v>31000.0</v>
@@ -1663,7 +1666,7 @@
         <v>2100.0</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="I19" t="n" s="0">
         <v>0.0</v>
@@ -1701,19 +1704,19 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F20" t="n" s="0">
         <v>30000.0</v>
@@ -1722,7 +1725,7 @@
         <v>2000.0</v>
       </c>
       <c r="H20" t="s" s="0">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="I20" t="n" s="0">
         <v>0.0</v>
@@ -1760,19 +1763,19 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s" s="0">
         <v>35</v>
-      </c>
-      <c r="D21" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s" s="0">
-        <v>23</v>
       </c>
       <c r="F21" t="n" s="0">
         <v>47000.0</v>
@@ -1781,7 +1784,7 @@
         <v>2400.0</v>
       </c>
       <c r="H21" t="s" s="0">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="I21" t="n" s="0">
         <v>0.0</v>
@@ -1819,28 +1822,28 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F22" t="n" s="0">
-        <v>45000.0</v>
+        <v>27000.0</v>
       </c>
       <c r="G22" t="n" s="0">
         <v>2200.0</v>
       </c>
       <c r="H22" t="s" s="0">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="I22" t="n" s="0">
         <v>0.0</v>
@@ -1864,7 +1867,7 @@
         <v>26</v>
       </c>
       <c r="P22" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="Q22" t="n" s="0">
         <v>0.0</v>
@@ -1878,52 +1881,52 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F23" t="n" s="0">
+        <v>32000.0</v>
+      </c>
+      <c r="G23" t="n" s="0">
+        <v>2300.0</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="I23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N23" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O23" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P23" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F23" t="n" s="0">
-        <v>27000.0</v>
-      </c>
-      <c r="G23" t="n" s="0">
-        <v>2200.0</v>
-      </c>
-      <c r="H23" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="I23" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J23" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K23" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L23" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M23" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N23" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O23" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P23" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q23" t="n" s="0">
         <v>0.0</v>
@@ -1937,28 +1940,28 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F24" t="n" s="0">
-        <v>31000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="G24" t="n" s="0">
-        <v>1900.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H24" t="s" s="0">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I24" t="n" s="0">
         <v>0.0</v>
@@ -1982,7 +1985,7 @@
         <v>26</v>
       </c>
       <c r="P24" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q24" t="n" s="0">
         <v>0.0</v>
@@ -1996,52 +1999,52 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F25" t="n" s="0">
+        <v>50000.0</v>
+      </c>
+      <c r="G25" t="n" s="0">
+        <v>2500.0</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="I25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N25" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O25" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P25" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F25" t="n" s="0">
-        <v>32000.0</v>
-      </c>
-      <c r="G25" t="n" s="0">
-        <v>2300.0</v>
-      </c>
-      <c r="H25" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="I25" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J25" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K25" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L25" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M25" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N25" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O25" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P25" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q25" t="n" s="0">
         <v>0.0</v>
@@ -2055,28 +2058,28 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F26" t="n" s="0">
-        <v>29000.0</v>
+        <v>36000.0</v>
       </c>
       <c r="G26" t="n" s="0">
-        <v>2100.0</v>
+        <v>2200.0</v>
       </c>
       <c r="H26" t="s" s="0">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="I26" t="n" s="0">
         <v>0.0</v>
@@ -2100,7 +2103,7 @@
         <v>26</v>
       </c>
       <c r="P26" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q26" t="n" s="0">
         <v>0.0</v>
@@ -2114,28 +2117,28 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F27" t="n" s="0">
-        <v>45000.0</v>
+        <v>24000.0</v>
       </c>
       <c r="G27" t="n" s="0">
-        <v>2400.0</v>
+        <v>2100.0</v>
       </c>
       <c r="H27" t="s" s="0">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="I27" t="n" s="0">
         <v>0.0</v>
@@ -2159,7 +2162,7 @@
         <v>26</v>
       </c>
       <c r="P27" t="s" s="0">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="Q27" t="n" s="0">
         <v>0.0</v>
@@ -2173,28 +2176,28 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F28" t="n" s="0">
-        <v>50000.0</v>
+        <v>41000.0</v>
       </c>
       <c r="G28" t="n" s="0">
-        <v>2500.0</v>
+        <v>2300.0</v>
       </c>
       <c r="H28" t="s" s="0">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="I28" t="n" s="0">
         <v>0.0</v>
@@ -2218,7 +2221,7 @@
         <v>26</v>
       </c>
       <c r="P28" t="s" s="0">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="Q28" t="n" s="0">
         <v>0.0</v>
@@ -2232,52 +2235,52 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E29" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F29" t="n" s="0">
+        <v>27000.0</v>
+      </c>
+      <c r="G29" t="n" s="0">
+        <v>1800.0</v>
+      </c>
+      <c r="H29" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="I29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N29" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O29" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P29" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F29" t="n" s="0">
-        <v>36000.0</v>
-      </c>
-      <c r="G29" t="n" s="0">
-        <v>2200.0</v>
-      </c>
-      <c r="H29" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="I29" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J29" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K29" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L29" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M29" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N29" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O29" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P29" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q29" t="n" s="0">
         <v>0.0</v>
@@ -2291,28 +2294,28 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F30" t="n" s="0">
-        <v>24000.0</v>
+        <v>38000.0</v>
       </c>
       <c r="G30" t="n" s="0">
-        <v>2100.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H30" t="s" s="0">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="I30" t="n" s="0">
         <v>0.0</v>
@@ -2336,7 +2339,7 @@
         <v>26</v>
       </c>
       <c r="P30" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q30" t="n" s="0">
         <v>0.0</v>
@@ -2350,52 +2353,52 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F31" t="n" s="0">
+        <v>45000.0</v>
+      </c>
+      <c r="G31" t="n" s="0">
+        <v>2000.0</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="I31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N31" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O31" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P31" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F31" t="n" s="0">
-        <v>41000.0</v>
-      </c>
-      <c r="G31" t="n" s="0">
-        <v>2300.0</v>
-      </c>
-      <c r="H31" t="s" s="0">
-        <v>117</v>
-      </c>
-      <c r="I31" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J31" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K31" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L31" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M31" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N31" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O31" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P31" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q31" t="n" s="0">
         <v>0.0</v>
@@ -2409,28 +2412,28 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F32" t="n" s="0">
-        <v>27000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="G32" t="n" s="0">
-        <v>1800.0</v>
+        <v>2100.0</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="I32" t="n" s="0">
         <v>0.0</v>
@@ -2454,7 +2457,7 @@
         <v>26</v>
       </c>
       <c r="P32" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q32" t="n" s="0">
         <v>0.0</v>
@@ -2468,52 +2471,52 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E33" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F33" t="n" s="0">
+        <v>33000.0</v>
+      </c>
+      <c r="G33" t="n" s="0">
+        <v>2200.0</v>
+      </c>
+      <c r="H33" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="I33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N33" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O33" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P33" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F33" t="n" s="0">
-        <v>38000.0</v>
-      </c>
-      <c r="G33" t="n" s="0">
-        <v>2400.0</v>
-      </c>
-      <c r="H33" t="s" s="0">
-        <v>123</v>
-      </c>
-      <c r="I33" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J33" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K33" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L33" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M33" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N33" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O33" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P33" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q33" t="n" s="0">
         <v>0.0</v>
@@ -2527,28 +2530,28 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E34" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F34" t="n" s="0">
-        <v>45000.0</v>
+        <v>49000.0</v>
       </c>
       <c r="G34" t="n" s="0">
-        <v>2000.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H34" t="s" s="0">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="I34" t="n" s="0">
         <v>0.0</v>
@@ -2572,7 +2575,7 @@
         <v>26</v>
       </c>
       <c r="P34" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q34" t="n" s="0">
         <v>0.0</v>
@@ -2586,28 +2589,28 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F35" t="n" s="0">
-        <v>25000.0</v>
+        <v>32000.0</v>
       </c>
       <c r="G35" t="n" s="0">
         <v>2100.0</v>
       </c>
       <c r="H35" t="s" s="0">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="I35" t="n" s="0">
         <v>0.0</v>
@@ -2631,7 +2634,7 @@
         <v>26</v>
       </c>
       <c r="P35" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q35" t="n" s="0">
         <v>0.0</v>
@@ -2645,28 +2648,28 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F36" t="n" s="0">
-        <v>33000.0</v>
+        <v>46000.0</v>
       </c>
       <c r="G36" t="n" s="0">
-        <v>2200.0</v>
+        <v>2300.0</v>
       </c>
       <c r="H36" t="s" s="0">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="I36" t="n" s="0">
         <v>0.0</v>
@@ -2690,7 +2693,7 @@
         <v>26</v>
       </c>
       <c r="P36" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q36" t="n" s="0">
         <v>0.0</v>
@@ -2704,52 +2707,52 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F37" t="n" s="0">
+        <v>29000.0</v>
+      </c>
+      <c r="G37" t="n" s="0">
+        <v>1800.0</v>
+      </c>
+      <c r="H37" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="I37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N37" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O37" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P37" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F37" t="n" s="0">
-        <v>49000.0</v>
-      </c>
-      <c r="G37" t="n" s="0">
-        <v>2400.0</v>
-      </c>
-      <c r="H37" t="s" s="0">
-        <v>135</v>
-      </c>
-      <c r="I37" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J37" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K37" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L37" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M37" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N37" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O37" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P37" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q37" t="n" s="0">
         <v>0.0</v>
@@ -2763,28 +2766,28 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E38" t="s" s="0">
         <v>23</v>
       </c>
       <c r="F38" t="n" s="0">
-        <v>32000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="G38" t="n" s="0">
-        <v>2100.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H38" t="s" s="0">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="I38" t="n" s="0">
         <v>0.0</v>
@@ -2808,7 +2811,7 @@
         <v>26</v>
       </c>
       <c r="P38" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q38" t="n" s="0">
         <v>0.0</v>
@@ -2822,52 +2825,52 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s" s="0">
         <v>43</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E39" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>37000.0</v>
+      </c>
+      <c r="G39" t="n" s="0">
+        <v>2100.0</v>
+      </c>
+      <c r="H39" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="I39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N39" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O39" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P39" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F39" t="n" s="0">
-        <v>46000.0</v>
-      </c>
-      <c r="G39" t="n" s="0">
-        <v>2300.0</v>
-      </c>
-      <c r="H39" t="s" s="0">
-        <v>140</v>
-      </c>
-      <c r="I39" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J39" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K39" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L39" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M39" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N39" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O39" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P39" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q39" t="n" s="0">
         <v>0.0</v>
@@ -2881,28 +2884,28 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F40" t="n" s="0">
-        <v>29000.0</v>
+        <v>48000.0</v>
       </c>
       <c r="G40" t="n" s="0">
-        <v>1800.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H40" t="s" s="0">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="I40" t="n" s="0">
         <v>0.0</v>
@@ -2926,7 +2929,7 @@
         <v>26</v>
       </c>
       <c r="P40" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q40" t="n" s="0">
         <v>0.0</v>
@@ -2940,28 +2943,28 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F41" t="n" s="0">
         <v>35000.0</v>
       </c>
       <c r="G41" t="n" s="0">
-        <v>2400.0</v>
+        <v>2300.0</v>
       </c>
       <c r="H41" t="s" s="0">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="I41" t="n" s="0">
         <v>0.0</v>
@@ -2985,7 +2988,7 @@
         <v>26</v>
       </c>
       <c r="P41" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q41" t="n" s="0">
         <v>0.0</v>
@@ -2999,28 +3002,28 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>56</v>
+        <v>159</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F42" t="n" s="0">
-        <v>37000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="G42" t="n" s="0">
-        <v>2100.0</v>
+        <v>2000.0</v>
       </c>
       <c r="H42" t="s" s="0">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="I42" t="n" s="0">
         <v>0.0</v>
@@ -3044,7 +3047,7 @@
         <v>26</v>
       </c>
       <c r="P42" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q42" t="n" s="0">
         <v>0.0</v>
@@ -3058,52 +3061,52 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E43" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F43" t="n" s="0">
+        <v>37000.0</v>
+      </c>
+      <c r="G43" t="n" s="0">
+        <v>2400.0</v>
+      </c>
+      <c r="H43" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="I43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N43" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O43" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P43" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F43" t="n" s="0">
-        <v>41000.0</v>
-      </c>
-      <c r="G43" t="n" s="0">
-        <v>2200.0</v>
-      </c>
-      <c r="H43" t="s" s="0">
-        <v>151</v>
-      </c>
-      <c r="I43" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J43" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K43" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L43" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M43" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N43" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O43" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P43" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q43" t="n" s="0">
         <v>0.0</v>
@@ -3117,28 +3120,28 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F44" t="n" s="0">
-        <v>48000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="G44" t="n" s="0">
-        <v>2400.0</v>
+        <v>2200.0</v>
       </c>
       <c r="H44" t="s" s="0">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="I44" t="n" s="0">
         <v>0.0</v>
@@ -3162,7 +3165,7 @@
         <v>26</v>
       </c>
       <c r="P44" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q44" t="n" s="0">
         <v>0.0</v>
@@ -3176,52 +3179,52 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E45" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F45" t="n" s="0">
+        <v>31000.0</v>
+      </c>
+      <c r="G45" t="n" s="0">
+        <v>2100.0</v>
+      </c>
+      <c r="H45" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="I45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N45" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O45" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="P45" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="F45" t="n" s="0">
-        <v>35000.0</v>
-      </c>
-      <c r="G45" t="n" s="0">
-        <v>2300.0</v>
-      </c>
-      <c r="H45" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="I45" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J45" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K45" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L45" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M45" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N45" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O45" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P45" t="s" s="0">
-        <v>92</v>
       </c>
       <c r="Q45" t="n" s="0">
         <v>0.0</v>
@@ -3235,28 +3238,28 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>160</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E46" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F46" t="n" s="0">
-        <v>30000.0</v>
+        <v>39000.0</v>
       </c>
       <c r="G46" t="n" s="0">
-        <v>2000.0</v>
+        <v>2400.0</v>
       </c>
       <c r="H46" t="s" s="0">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I46" t="n" s="0">
         <v>0.0</v>
@@ -3280,7 +3283,7 @@
         <v>26</v>
       </c>
       <c r="P46" t="s" s="0">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q46" t="n" s="0">
         <v>0.0</v>
@@ -3289,242 +3292,6 @@
         <v>0.0</v>
       </c>
       <c r="S46" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
-        <v>162</v>
-      </c>
-      <c r="B47" t="s" s="0">
-        <v>163</v>
-      </c>
-      <c r="C47" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="D47" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E47" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F47" t="n" s="0">
-        <v>37000.0</v>
-      </c>
-      <c r="G47" t="n" s="0">
-        <v>2400.0</v>
-      </c>
-      <c r="H47" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="I47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N47" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O47" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P47" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="Q47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R47" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="S47" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="B48" t="s" s="0">
-        <v>165</v>
-      </c>
-      <c r="C48" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="D48" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E48" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F48" t="n" s="0">
-        <v>45000.0</v>
-      </c>
-      <c r="G48" t="n" s="0">
-        <v>2200.0</v>
-      </c>
-      <c r="H48" t="s" s="0">
-        <v>166</v>
-      </c>
-      <c r="I48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N48" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O48" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P48" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="Q48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R48" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="S48" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="0">
-        <v>167</v>
-      </c>
-      <c r="B49" t="s" s="0">
-        <v>168</v>
-      </c>
-      <c r="C49" t="s" s="0">
-        <v>169</v>
-      </c>
-      <c r="D49" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E49" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F49" t="n" s="0">
-        <v>31000.0</v>
-      </c>
-      <c r="G49" t="n" s="0">
-        <v>2100.0</v>
-      </c>
-      <c r="H49" t="s" s="0">
-        <v>170</v>
-      </c>
-      <c r="I49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N49" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O49" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P49" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="Q49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R49" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="S49" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="B50" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="C50" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D50" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E50" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F50" t="n" s="0">
-        <v>39000.0</v>
-      </c>
-      <c r="G50" t="n" s="0">
-        <v>2400.0</v>
-      </c>
-      <c r="H50" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="I50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N50" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O50" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="P50" t="s" s="0">
-        <v>92</v>
-      </c>
-      <c r="Q50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R50" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="S50" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimizacion de diseños y procesos No.12
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170C519F-DC34-4254-B8BC-280415DA6009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360CCDD5-0C41-4B9A-B8CB-2CAC595CDC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="168">
   <si>
     <t>Placas</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Isuzu</t>
   </si>
   <si>
-    <t>INACTIVO</t>
-  </si>
-  <si>
     <t>Diésel</t>
   </si>
   <si>
@@ -100,12 +97,6 @@
     <t/>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>31/12/1899</t>
-  </si>
-  <si>
     <t>PQR345</t>
   </si>
   <si>
@@ -367,9 +358,6 @@
     <t>05/08/2016</t>
   </si>
   <si>
-    <t>12/10/2024</t>
-  </si>
-  <si>
     <t>YZA567</t>
   </si>
   <si>
@@ -379,9 +367,6 @@
     <t>15/09/2017</t>
   </si>
   <si>
-    <t>Ninguno</t>
-  </si>
-  <si>
     <t>BCD890</t>
   </si>
   <si>
@@ -509,9 +494,6 @@
   </si>
   <si>
     <t>Z270</t>
-  </si>
-  <si>
-    <t>DESCOMPUESTO</t>
   </si>
   <si>
     <t>10/07/2018</t>
@@ -915,12 +897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D2:D46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -992,10 +973,10 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
       </c>
       <c r="F2">
         <v>41000</v>
@@ -1004,7 +985,7 @@
         <v>2200</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1022,13 +1003,13 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1037,24 +1018,24 @@
         <v>0</v>
       </c>
       <c r="S2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
       </c>
       <c r="F3">
         <v>47000</v>
@@ -1063,7 +1044,7 @@
         <v>2400</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1081,13 +1062,13 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1096,24 +1077,24 @@
         <v>0</v>
       </c>
       <c r="S3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>45000</v>
@@ -1122,7 +1103,7 @@
         <v>2200</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1140,13 +1121,13 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1160,19 +1141,19 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>29000</v>
@@ -1181,7 +1162,7 @@
         <v>2100</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1199,13 +1180,13 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1219,19 +1200,19 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <v>28000</v>
@@ -1240,7 +1221,7 @@
         <v>1600</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1258,13 +1239,13 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1278,19 +1259,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>15000</v>
@@ -1299,7 +1280,7 @@
         <v>1900</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1317,13 +1298,13 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1337,19 +1318,19 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8">
         <v>31000</v>
@@ -1358,7 +1339,7 @@
         <v>1900</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1376,13 +1357,13 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1396,19 +1377,19 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9">
         <v>31000</v>
@@ -1417,7 +1398,7 @@
         <v>2000</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1435,13 +1416,13 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1455,19 +1436,19 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10">
         <v>38000</v>
@@ -1476,7 +1457,7 @@
         <v>2100</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1494,13 +1475,13 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1514,19 +1495,19 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>63</v>
       </c>
       <c r="F11">
         <v>26000</v>
@@ -1535,7 +1516,7 @@
         <v>1800</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1553,13 +1534,13 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1573,19 +1554,19 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
         <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
       </c>
       <c r="F12">
         <v>45000</v>
@@ -1594,7 +1575,7 @@
         <v>2500</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1612,13 +1593,13 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1632,19 +1613,19 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>27000</v>
@@ -1653,7 +1634,7 @@
         <v>2300</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1671,13 +1652,13 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1691,19 +1672,19 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>40000</v>
@@ -1712,7 +1693,7 @@
         <v>2100</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1730,13 +1711,13 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1750,19 +1731,19 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>34000</v>
@@ -1771,7 +1752,7 @@
         <v>2200</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1789,13 +1770,13 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1809,19 +1790,19 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16">
         <v>32000</v>
@@ -1830,7 +1811,7 @@
         <v>1900</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1848,13 +1829,13 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1868,19 +1849,19 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F17">
         <v>31000</v>
@@ -1889,7 +1870,7 @@
         <v>2000</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1907,13 +1888,13 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1927,19 +1908,19 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F18">
         <v>32000</v>
@@ -1948,7 +1929,7 @@
         <v>1700</v>
       </c>
       <c r="H18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1966,13 +1947,13 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1986,19 +1967,19 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19">
         <v>31000</v>
@@ -2007,7 +1988,7 @@
         <v>2100</v>
       </c>
       <c r="H19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2025,13 +2006,13 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2045,19 +2026,19 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F20">
         <v>30000</v>
@@ -2066,7 +2047,7 @@
         <v>2000</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2084,13 +2065,13 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2104,19 +2085,19 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F21">
         <v>47000</v>
@@ -2125,7 +2106,7 @@
         <v>2400</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2143,13 +2124,13 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -2163,19 +2144,19 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22">
         <v>27000</v>
@@ -2184,7 +2165,7 @@
         <v>2200</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2202,13 +2183,13 @@
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2222,19 +2203,19 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23">
         <v>32000</v>
@@ -2243,7 +2224,7 @@
         <v>2300</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2261,13 +2242,13 @@
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -2281,19 +2262,19 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24">
         <v>45000</v>
@@ -2302,7 +2283,7 @@
         <v>2400</v>
       </c>
       <c r="H24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2320,13 +2301,13 @@
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -2340,19 +2321,19 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F25">
         <v>50000</v>
@@ -2361,7 +2342,7 @@
         <v>2500</v>
       </c>
       <c r="H25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2379,13 +2360,13 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -2399,19 +2380,19 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26">
         <v>36000</v>
@@ -2420,7 +2401,7 @@
         <v>2200</v>
       </c>
       <c r="H26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2438,13 +2419,13 @@
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2458,19 +2439,19 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F27">
         <v>24000</v>
@@ -2479,7 +2460,7 @@
         <v>2100</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2497,13 +2478,13 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P27" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -2517,19 +2498,19 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F28">
         <v>41000</v>
@@ -2538,7 +2519,7 @@
         <v>2300</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2556,13 +2537,13 @@
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P28" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -2576,19 +2557,19 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F29">
         <v>27000</v>
@@ -2597,7 +2578,7 @@
         <v>1800</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2615,13 +2596,13 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2635,19 +2616,19 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30">
         <v>38000</v>
@@ -2656,7 +2637,7 @@
         <v>2400</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2674,13 +2655,13 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -2694,19 +2675,19 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
         <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F31">
         <v>45000</v>
@@ -2715,7 +2696,7 @@
         <v>2000</v>
       </c>
       <c r="H31" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2733,13 +2714,13 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -2753,19 +2734,19 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F32">
         <v>25000</v>
@@ -2774,7 +2755,7 @@
         <v>2100</v>
       </c>
       <c r="H32" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2792,13 +2773,13 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q32">
         <v>0</v>
@@ -2812,19 +2793,19 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F33">
         <v>33000</v>
@@ -2833,7 +2814,7 @@
         <v>2200</v>
       </c>
       <c r="H33" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2851,13 +2832,13 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P33" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q33">
         <v>0</v>
@@ -2871,19 +2852,19 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F34">
         <v>49000</v>
@@ -2892,7 +2873,7 @@
         <v>2400</v>
       </c>
       <c r="H34" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2910,13 +2891,13 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P34" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -2930,19 +2911,19 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F35">
         <v>32000</v>
@@ -2951,7 +2932,7 @@
         <v>2100</v>
       </c>
       <c r="H35" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2969,13 +2950,13 @@
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q35">
         <v>0</v>
@@ -2989,19 +2970,19 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F36">
         <v>46000</v>
@@ -3010,7 +2991,7 @@
         <v>2300</v>
       </c>
       <c r="H36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -3028,13 +3009,13 @@
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -3048,19 +3029,19 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F37">
         <v>29000</v>
@@ -3069,7 +3050,7 @@
         <v>1800</v>
       </c>
       <c r="H37" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3087,13 +3068,13 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q37">
         <v>0</v>
@@ -3107,19 +3088,19 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F38">
         <v>35000</v>
@@ -3128,7 +3109,7 @@
         <v>2400</v>
       </c>
       <c r="H38" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -3146,13 +3127,13 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P38" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -3166,19 +3147,19 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F39">
         <v>37000</v>
@@ -3187,7 +3168,7 @@
         <v>2100</v>
       </c>
       <c r="H39" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -3205,13 +3186,13 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P39" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q39">
         <v>0</v>
@@ -3225,19 +3206,19 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F40">
         <v>48000</v>
@@ -3246,7 +3227,7 @@
         <v>2400</v>
       </c>
       <c r="H40" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -3264,13 +3245,13 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q40">
         <v>0</v>
@@ -3284,19 +3265,19 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F41">
         <v>35000</v>
@@ -3305,10 +3286,10 @@
         <v>2300</v>
       </c>
       <c r="H41" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I41">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -3323,16 +3304,16 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q41">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="R41">
         <v>0</v>
@@ -3343,19 +3324,19 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F42">
         <v>30000</v>
@@ -3364,16 +3345,16 @@
         <v>2000</v>
       </c>
       <c r="H42" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K42">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L42">
         <v>0</v>
@@ -3382,19 +3363,19 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q42">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="R42">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="S42" t="b">
         <v>1</v>
@@ -3402,19 +3383,19 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="E43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F43">
         <v>37000</v>
@@ -3423,7 +3404,7 @@
         <v>2400</v>
       </c>
       <c r="H43" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -3441,13 +3422,13 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q43">
         <v>0</v>
@@ -3461,19 +3442,19 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F44">
         <v>45000</v>
@@ -3482,7 +3463,7 @@
         <v>2200</v>
       </c>
       <c r="H44" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -3500,13 +3481,13 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -3520,19 +3501,19 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F45">
         <v>31000</v>
@@ -3541,7 +3522,7 @@
         <v>2100</v>
       </c>
       <c r="H45" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -3559,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P45" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q45">
         <v>0</v>
@@ -3579,19 +3560,19 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E46" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F46">
         <v>39000</v>
@@ -3600,7 +3581,7 @@
         <v>2400</v>
       </c>
       <c r="H46" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -3618,13 +3599,13 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q46">
         <v>0</v>

</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑO E INTERFACES NO.13
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONES.xlsx
+++ b/ProyectoPooDist/excels/CAMIONES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360CCDD5-0C41-4B9A-B8CB-2CAC595CDC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FAE727-F4F5-4DBF-B281-84FA002D7767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="194">
   <si>
     <t>Placas</t>
   </si>
@@ -79,432 +79,444 @@
     <t>Activo</t>
   </si>
   <si>
+    <t>JKL012</t>
+  </si>
+  <si>
+    <t>D400</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>INACTIVO</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>30/10/2020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>STU456</t>
+  </si>
+  <si>
+    <t>X16</t>
+  </si>
+  <si>
+    <t>Rex</t>
+  </si>
+  <si>
+    <t>Eléctrico</t>
+  </si>
+  <si>
+    <t>24/10/2019</t>
+  </si>
+  <si>
+    <t>EFG234</t>
+  </si>
+  <si>
+    <t>K1100</t>
+  </si>
+  <si>
+    <t>Hino</t>
+  </si>
+  <si>
+    <t>Diésel</t>
+  </si>
+  <si>
+    <t>12/06/2019</t>
+  </si>
+  <si>
     <t>DEF234</t>
   </si>
   <si>
     <t>U2100</t>
   </si>
   <si>
+    <t>Ryax</t>
+  </si>
+  <si>
+    <t>FUNCIONAL</t>
+  </si>
+  <si>
+    <t>Disel</t>
+  </si>
+  <si>
+    <t>30/09/2017</t>
+  </si>
+  <si>
+    <t>PQR345</t>
+  </si>
+  <si>
+    <t>X15</t>
+  </si>
+  <si>
+    <t>Yumeku</t>
+  </si>
+  <si>
+    <t>29/10/2017</t>
+  </si>
+  <si>
+    <t>ABC345</t>
+  </si>
+  <si>
+    <t>X24</t>
+  </si>
+  <si>
+    <t>Iveco</t>
+  </si>
+  <si>
+    <t>27/10/2015</t>
+  </si>
+  <si>
+    <t>EFG456</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>Kenworth</t>
+  </si>
+  <si>
+    <t>21/10/2015</t>
+  </si>
+  <si>
+    <t>EFG123</t>
+  </si>
+  <si>
+    <t>Scania</t>
+  </si>
+  <si>
+    <t>26/10/2017</t>
+  </si>
+  <si>
+    <t>DEF456</t>
+  </si>
+  <si>
+    <t>B200</t>
+  </si>
+  <si>
+    <t>22/06/2018</t>
+  </si>
+  <si>
+    <t>DEF890</t>
+  </si>
+  <si>
+    <t>X20</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>28/10/2016</t>
+  </si>
+  <si>
+    <t>VWX567</t>
+  </si>
+  <si>
+    <t>X17</t>
+  </si>
+  <si>
+    <t>26/10/2018</t>
+  </si>
+  <si>
+    <t>GHI012</t>
+  </si>
+  <si>
+    <t>MEME</t>
+  </si>
+  <si>
+    <t>Nissa</t>
+  </si>
+  <si>
+    <t>ABC789</t>
+  </si>
+  <si>
+    <t>X19</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>23/10/2017</t>
+  </si>
+  <si>
+    <t>HIJ456</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>27/10/2018</t>
+  </si>
+  <si>
+    <t>XYZ678</t>
+  </si>
+  <si>
+    <t>X18</t>
+  </si>
+  <si>
+    <t>MNO234</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>25/10/2014</t>
+  </si>
+  <si>
+    <t>STU789</t>
+  </si>
+  <si>
+    <t>22/10/2016</t>
+  </si>
+  <si>
+    <t>HIJ789</t>
+  </si>
+  <si>
+    <t>23/10/2014</t>
+  </si>
+  <si>
+    <t>VWX123</t>
+  </si>
+  <si>
+    <t>X21</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>DEF123</t>
+  </si>
+  <si>
+    <t>X22</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>GHI123</t>
+  </si>
+  <si>
+    <t>X23</t>
+  </si>
+  <si>
+    <t>XYZ123</t>
+  </si>
+  <si>
+    <t>A100</t>
+  </si>
+  <si>
     <t>Isuzu</t>
   </si>
   <si>
-    <t>Diésel</t>
-  </si>
-  <si>
-    <t>30/09/2017</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PQR345</t>
-  </si>
-  <si>
-    <t>X15</t>
+    <t>12/04/2019</t>
+  </si>
+  <si>
+    <t>GHI789</t>
+  </si>
+  <si>
+    <t>C300</t>
+  </si>
+  <si>
+    <t>Freightliner</t>
+  </si>
+  <si>
+    <t>14/09/2017</t>
+  </si>
+  <si>
+    <t>MNO345</t>
+  </si>
+  <si>
+    <t>E500</t>
+  </si>
+  <si>
+    <t>28/02/2016</t>
+  </si>
+  <si>
+    <t>PQR678</t>
+  </si>
+  <si>
+    <t>F600</t>
+  </si>
+  <si>
+    <t>Mack</t>
+  </si>
+  <si>
+    <t>15/11/2018</t>
+  </si>
+  <si>
+    <t>STU901</t>
+  </si>
+  <si>
+    <t>G700</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>20/03/2019</t>
+  </si>
+  <si>
+    <t>VWX234</t>
+  </si>
+  <si>
+    <t>H800</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>05/08/2016</t>
+  </si>
+  <si>
+    <t>YZA567</t>
+  </si>
+  <si>
+    <t>I900</t>
+  </si>
+  <si>
+    <t>15/09/2017</t>
+  </si>
+  <si>
+    <t>BCD890</t>
+  </si>
+  <si>
+    <t>J1000</t>
+  </si>
+  <si>
+    <t>22/01/2020</t>
+  </si>
+  <si>
+    <t>GHI567</t>
+  </si>
+  <si>
+    <t>L1200</t>
+  </si>
+  <si>
+    <t>30/04/2018</t>
+  </si>
+  <si>
+    <t>JKL890</t>
+  </si>
+  <si>
+    <t>M1300</t>
+  </si>
+  <si>
+    <t>10/02/2021</t>
+  </si>
+  <si>
+    <t>NOP123</t>
+  </si>
+  <si>
+    <t>N1400</t>
+  </si>
+  <si>
+    <t>01/07/2016</t>
+  </si>
+  <si>
+    <t>QRS456</t>
+  </si>
+  <si>
+    <t>O1500</t>
+  </si>
+  <si>
+    <t>15/11/2019</t>
+  </si>
+  <si>
+    <t>P1600</t>
+  </si>
+  <si>
+    <t>20/05/2017</t>
+  </si>
+  <si>
+    <t>TUV012</t>
+  </si>
+  <si>
+    <t>1700.0</t>
+  </si>
+  <si>
+    <t>10/03/2018</t>
+  </si>
+  <si>
+    <t>VWX345</t>
+  </si>
+  <si>
+    <t>R1800</t>
+  </si>
+  <si>
+    <t>01/01/2016</t>
+  </si>
+  <si>
+    <t>S1900</t>
+  </si>
+  <si>
+    <t>22/04/2020</t>
+  </si>
+  <si>
+    <t>ABC901</t>
+  </si>
+  <si>
+    <t>T2000</t>
+  </si>
+  <si>
+    <t>15/08/2019</t>
+  </si>
+  <si>
+    <t>V2200</t>
+  </si>
+  <si>
+    <t>12/02/2018</t>
+  </si>
+  <si>
+    <t>XYZ234</t>
+  </si>
+  <si>
+    <t>X250</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>14/03/2020</t>
+  </si>
+  <si>
+    <t>DEF567</t>
+  </si>
+  <si>
+    <t>Y260</t>
+  </si>
+  <si>
+    <t>Fuso</t>
+  </si>
+  <si>
+    <t>22/05/2019</t>
+  </si>
+  <si>
+    <t>GHI890</t>
+  </si>
+  <si>
+    <t>Z270</t>
+  </si>
+  <si>
+    <t>10/07/2018</t>
+  </si>
+  <si>
+    <t>JKL123</t>
+  </si>
+  <si>
+    <t>A280</t>
   </si>
   <si>
     <t>MAN</t>
   </si>
   <si>
-    <t>Gasolina</t>
-  </si>
-  <si>
-    <t>29/10/2017</t>
-  </si>
-  <si>
-    <t>ABC345</t>
-  </si>
-  <si>
-    <t>X24</t>
-  </si>
-  <si>
-    <t>Iveco</t>
-  </si>
-  <si>
-    <t>FUNCIONAL</t>
-  </si>
-  <si>
-    <t>27/10/2015</t>
-  </si>
-  <si>
-    <t>JKL012</t>
-  </si>
-  <si>
-    <t>D400</t>
-  </si>
-  <si>
-    <t>Mitsubishi</t>
-  </si>
-  <si>
-    <t>30/10/2020</t>
-  </si>
-  <si>
-    <t>EFG456</t>
-  </si>
-  <si>
-    <t>X11</t>
-  </si>
-  <si>
-    <t>Kenworth</t>
-  </si>
-  <si>
-    <t>21/10/2015</t>
-  </si>
-  <si>
-    <t>EFG123</t>
-  </si>
-  <si>
-    <t>Scania</t>
-  </si>
-  <si>
-    <t>26/10/2017</t>
-  </si>
-  <si>
-    <t>DEF456</t>
-  </si>
-  <si>
-    <t>B200</t>
-  </si>
-  <si>
-    <t>Hino</t>
-  </si>
-  <si>
-    <t>22/06/2018</t>
-  </si>
-  <si>
-    <t>DEF890</t>
-  </si>
-  <si>
-    <t>X20</t>
-  </si>
-  <si>
-    <t>Renault</t>
-  </si>
-  <si>
-    <t>28/10/2016</t>
-  </si>
-  <si>
-    <t>VWX567</t>
-  </si>
-  <si>
-    <t>X17</t>
-  </si>
-  <si>
-    <t>26/10/2018</t>
-  </si>
-  <si>
-    <t>STU456</t>
-  </si>
-  <si>
-    <t>X16</t>
-  </si>
-  <si>
-    <t>Volvo</t>
-  </si>
-  <si>
-    <t>Eléctrico</t>
-  </si>
-  <si>
-    <t>24/10/2019</t>
-  </si>
-  <si>
-    <t>GHI012</t>
-  </si>
-  <si>
-    <t>MEME</t>
-  </si>
-  <si>
-    <t>Nissa</t>
-  </si>
-  <si>
-    <t>Disel</t>
-  </si>
-  <si>
-    <t>ABC789</t>
-  </si>
-  <si>
-    <t>X19</t>
-  </si>
-  <si>
-    <t>Mercedes</t>
-  </si>
-  <si>
-    <t>23/10/2017</t>
-  </si>
-  <si>
-    <t>HIJ456</t>
-  </si>
-  <si>
-    <t>X12</t>
-  </si>
-  <si>
-    <t>27/10/2018</t>
-  </si>
-  <si>
-    <t>XYZ678</t>
-  </si>
-  <si>
-    <t>X18</t>
-  </si>
-  <si>
-    <t>MNO234</t>
-  </si>
-  <si>
-    <t>X14</t>
-  </si>
-  <si>
-    <t>25/10/2014</t>
-  </si>
-  <si>
-    <t>STU789</t>
-  </si>
-  <si>
-    <t>22/10/2016</t>
-  </si>
-  <si>
-    <t>HIJ789</t>
-  </si>
-  <si>
-    <t>23/10/2014</t>
-  </si>
-  <si>
-    <t>VWX123</t>
-  </si>
-  <si>
-    <t>X21</t>
-  </si>
-  <si>
-    <t>Ford</t>
-  </si>
-  <si>
-    <t>DEF123</t>
-  </si>
-  <si>
-    <t>X22</t>
-  </si>
-  <si>
-    <t>Toyota</t>
-  </si>
-  <si>
-    <t>GHI123</t>
-  </si>
-  <si>
-    <t>X23</t>
-  </si>
-  <si>
-    <t>XYZ123</t>
-  </si>
-  <si>
-    <t>A100</t>
-  </si>
-  <si>
-    <t>12/04/2019</t>
-  </si>
-  <si>
-    <t>GHI789</t>
-  </si>
-  <si>
-    <t>C300</t>
-  </si>
-  <si>
-    <t>Freightliner</t>
-  </si>
-  <si>
-    <t>14/09/2017</t>
-  </si>
-  <si>
-    <t>MNO345</t>
-  </si>
-  <si>
-    <t>E500</t>
-  </si>
-  <si>
-    <t>28/02/2016</t>
-  </si>
-  <si>
-    <t>PQR678</t>
-  </si>
-  <si>
-    <t>F600</t>
-  </si>
-  <si>
-    <t>Mack</t>
-  </si>
-  <si>
-    <t>15/11/2018</t>
-  </si>
-  <si>
-    <t>STU901</t>
-  </si>
-  <si>
-    <t>G700</t>
-  </si>
-  <si>
-    <t>International</t>
-  </si>
-  <si>
-    <t>20/03/2019</t>
-  </si>
-  <si>
-    <t>VWX234</t>
-  </si>
-  <si>
-    <t>H800</t>
-  </si>
-  <si>
-    <t>Nissan</t>
-  </si>
-  <si>
-    <t>05/08/2016</t>
-  </si>
-  <si>
-    <t>YZA567</t>
-  </si>
-  <si>
-    <t>I900</t>
-  </si>
-  <si>
-    <t>15/09/2017</t>
-  </si>
-  <si>
-    <t>BCD890</t>
-  </si>
-  <si>
-    <t>J1000</t>
-  </si>
-  <si>
-    <t>22/01/2020</t>
-  </si>
-  <si>
-    <t>EFG234</t>
-  </si>
-  <si>
-    <t>K1100</t>
-  </si>
-  <si>
-    <t>12/06/2019</t>
-  </si>
-  <si>
-    <t>GHI567</t>
-  </si>
-  <si>
-    <t>L1200</t>
-  </si>
-  <si>
-    <t>30/04/2018</t>
-  </si>
-  <si>
-    <t>JKL890</t>
-  </si>
-  <si>
-    <t>M1300</t>
-  </si>
-  <si>
-    <t>10/02/2021</t>
-  </si>
-  <si>
-    <t>NOP123</t>
-  </si>
-  <si>
-    <t>N1400</t>
-  </si>
-  <si>
-    <t>01/07/2016</t>
-  </si>
-  <si>
-    <t>QRS456</t>
-  </si>
-  <si>
-    <t>O1500</t>
-  </si>
-  <si>
-    <t>15/11/2019</t>
-  </si>
-  <si>
-    <t>P1600</t>
-  </si>
-  <si>
-    <t>20/05/2017</t>
-  </si>
-  <si>
-    <t>TUV012</t>
-  </si>
-  <si>
-    <t>1700.0</t>
-  </si>
-  <si>
-    <t>10/03/2018</t>
-  </si>
-  <si>
-    <t>VWX345</t>
-  </si>
-  <si>
-    <t>R1800</t>
-  </si>
-  <si>
-    <t>01/01/2016</t>
-  </si>
-  <si>
-    <t>S1900</t>
-  </si>
-  <si>
-    <t>22/04/2020</t>
-  </si>
-  <si>
-    <t>ABC901</t>
-  </si>
-  <si>
-    <t>T2000</t>
-  </si>
-  <si>
-    <t>15/08/2019</t>
-  </si>
-  <si>
-    <t>V2200</t>
-  </si>
-  <si>
-    <t>12/02/2018</t>
-  </si>
-  <si>
-    <t>XYZ234</t>
-  </si>
-  <si>
-    <t>X250</t>
-  </si>
-  <si>
-    <t>Tata</t>
-  </si>
-  <si>
-    <t>14/03/2020</t>
-  </si>
-  <si>
-    <t>DEF567</t>
-  </si>
-  <si>
-    <t>Y260</t>
-  </si>
-  <si>
-    <t>Fuso</t>
-  </si>
-  <si>
-    <t>22/05/2019</t>
-  </si>
-  <si>
-    <t>GHI890</t>
-  </si>
-  <si>
-    <t>Z270</t>
-  </si>
-  <si>
-    <t>10/07/2018</t>
-  </si>
-  <si>
-    <t>JKL123</t>
-  </si>
-  <si>
-    <t>A280</t>
-  </si>
-  <si>
     <t>18/10/2021</t>
   </si>
   <si>
@@ -524,6 +536,72 @@
   </si>
   <si>
     <t>05/02/2019</t>
+  </si>
+  <si>
+    <t>ASDSA1</t>
+  </si>
+  <si>
+    <t>Versa</t>
+  </si>
+  <si>
+    <t>16/07/1905</t>
+  </si>
+  <si>
+    <t>ASDSAD1</t>
+  </si>
+  <si>
+    <t>321j</t>
+  </si>
+  <si>
+    <t>nisssa</t>
+  </si>
+  <si>
+    <t>AS12</t>
+  </si>
+  <si>
+    <t>SADSA1</t>
+  </si>
+  <si>
+    <t>NISSAA</t>
+  </si>
+  <si>
+    <t>DSA21</t>
+  </si>
+  <si>
+    <t>S122</t>
+  </si>
+  <si>
+    <t>ASD1</t>
+  </si>
+  <si>
+    <t>SAD1</t>
+  </si>
+  <si>
+    <t>P123GRV</t>
+  </si>
+  <si>
+    <t>Cs</t>
+  </si>
+  <si>
+    <t>31/05/1905</t>
+  </si>
+  <si>
+    <t>P021WWH</t>
+  </si>
+  <si>
+    <t>VOLVO</t>
+  </si>
+  <si>
+    <t>NISSAN</t>
+  </si>
+  <si>
+    <t>12/07/1905</t>
+  </si>
+  <si>
+    <t>ASD12</t>
+  </si>
+  <si>
+    <t>SAD12</t>
   </si>
 </sst>
 </file>
@@ -895,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D2:D46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,19 +1051,19 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2">
-        <v>41000</v>
+        <v>29000</v>
       </c>
       <c r="G2">
-        <v>2200</v>
+        <v>2100</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1003,13 +1081,13 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1023,28 +1101,28 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3">
-        <v>47000</v>
+        <v>26000</v>
       </c>
       <c r="G3">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1062,13 +1140,13 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1082,28 +1160,28 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F4">
-        <v>45000</v>
+        <v>38000</v>
       </c>
       <c r="G4">
-        <v>2200</v>
+        <v>2400</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1121,13 +1199,13 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1141,28 +1219,28 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F5">
-        <v>29000</v>
+        <v>41000</v>
       </c>
       <c r="G5">
-        <v>2100</v>
+        <v>2200</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1180,13 +1258,13 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1200,28 +1278,28 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6">
-        <v>28000</v>
+        <v>47000</v>
       </c>
       <c r="G6">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1239,13 +1317,13 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1259,28 +1337,28 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F7">
-        <v>15000</v>
+        <v>45000</v>
       </c>
       <c r="G7">
-        <v>1900</v>
+        <v>2200</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1298,13 +1376,13 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1318,28 +1396,28 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8">
-        <v>31000</v>
+        <v>28000</v>
       </c>
       <c r="G8">
-        <v>1900</v>
+        <v>1600</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1357,13 +1435,13 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1377,28 +1455,28 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F9">
-        <v>31000</v>
+        <v>15000</v>
       </c>
       <c r="G9">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1416,13 +1494,13 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1436,28 +1514,28 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>38000</v>
+        <v>31000</v>
       </c>
       <c r="G10">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1475,13 +1553,13 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1495,28 +1573,28 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="F11">
-        <v>26000</v>
+        <v>31000</v>
       </c>
       <c r="G11">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1534,13 +1612,13 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1554,28 +1632,28 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="F12">
-        <v>45000</v>
+        <v>38000</v>
       </c>
       <c r="G12">
-        <v>2500</v>
+        <v>2100</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1593,13 +1671,13 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1613,28 +1691,28 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F13">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="G13">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1652,13 +1730,13 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1678,22 +1756,22 @@
         <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F14">
-        <v>40000</v>
+        <v>27000</v>
       </c>
       <c r="G14">
-        <v>2100</v>
+        <v>2300</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1711,13 +1789,13 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1731,28 +1809,28 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>34000</v>
+        <v>40000</v>
       </c>
       <c r="G15">
-        <v>2200</v>
+        <v>2100</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1770,13 +1848,13 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1790,28 +1868,28 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F16">
-        <v>32000</v>
+        <v>34000</v>
       </c>
       <c r="G16">
-        <v>1900</v>
+        <v>2200</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1829,13 +1907,13 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1849,28 +1927,28 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F17">
-        <v>31000</v>
+        <v>32000</v>
       </c>
       <c r="G17">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1888,13 +1966,13 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1908,28 +1986,28 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F18">
-        <v>32000</v>
+        <v>31000</v>
       </c>
       <c r="G18">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1947,13 +2025,13 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1967,28 +2045,28 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19">
-        <v>31000</v>
+        <v>32000</v>
       </c>
       <c r="G19">
-        <v>2100</v>
+        <v>1700</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2006,13 +2084,13 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2026,28 +2104,28 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F20">
-        <v>30000</v>
+        <v>31000</v>
       </c>
       <c r="G20">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2065,13 +2143,13 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2085,28 +2163,28 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F21">
-        <v>47000</v>
+        <v>30000</v>
       </c>
       <c r="G21">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2124,13 +2202,13 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -2144,28 +2222,28 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F22">
-        <v>27000</v>
+        <v>47000</v>
       </c>
       <c r="G22">
-        <v>2200</v>
+        <v>2400</v>
       </c>
       <c r="H22" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2183,13 +2261,13 @@
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2203,28 +2281,28 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F23">
-        <v>32000</v>
+        <v>27000</v>
       </c>
       <c r="G23">
-        <v>2300</v>
+        <v>2200</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2242,13 +2320,13 @@
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -2262,28 +2340,28 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F24">
-        <v>45000</v>
+        <v>32000</v>
       </c>
       <c r="G24">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="H24" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2301,13 +2379,13 @@
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -2321,28 +2399,28 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F25">
-        <v>50000</v>
+        <v>45000</v>
       </c>
       <c r="G25">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2360,13 +2438,13 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -2380,28 +2458,28 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F26">
-        <v>36000</v>
+        <v>50000</v>
       </c>
       <c r="G26">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2419,13 +2497,13 @@
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2439,28 +2517,28 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F27">
-        <v>24000</v>
+        <v>36000</v>
       </c>
       <c r="G27">
-        <v>2100</v>
+        <v>2200</v>
       </c>
       <c r="H27" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2478,13 +2556,13 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -2498,28 +2576,28 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F28">
-        <v>41000</v>
+        <v>24000</v>
       </c>
       <c r="G28">
-        <v>2300</v>
+        <v>2100</v>
       </c>
       <c r="H28" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2537,13 +2615,13 @@
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -2557,28 +2635,28 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F29">
-        <v>27000</v>
+        <v>41000</v>
       </c>
       <c r="G29">
-        <v>1800</v>
+        <v>2300</v>
       </c>
       <c r="H29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2596,13 +2674,13 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2616,28 +2694,28 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F30">
-        <v>38000</v>
+        <v>27000</v>
       </c>
       <c r="G30">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="H30" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2655,13 +2733,13 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -2675,19 +2753,19 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F31">
         <v>45000</v>
@@ -2696,7 +2774,7 @@
         <v>2000</v>
       </c>
       <c r="H31" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2714,13 +2792,13 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -2734,19 +2812,19 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F32">
         <v>25000</v>
@@ -2755,7 +2833,7 @@
         <v>2100</v>
       </c>
       <c r="H32" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2773,13 +2851,13 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q32">
         <v>0</v>
@@ -2793,19 +2871,19 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F33">
         <v>33000</v>
@@ -2814,7 +2892,7 @@
         <v>2200</v>
       </c>
       <c r="H33" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2832,13 +2910,13 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q33">
         <v>0</v>
@@ -2852,19 +2930,19 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F34">
         <v>49000</v>
@@ -2873,7 +2951,7 @@
         <v>2400</v>
       </c>
       <c r="H34" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2891,13 +2969,13 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -2911,19 +2989,19 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F35">
         <v>32000</v>
@@ -2932,7 +3010,7 @@
         <v>2100</v>
       </c>
       <c r="H35" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2950,13 +3028,13 @@
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q35">
         <v>0</v>
@@ -2970,19 +3048,19 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F36">
         <v>46000</v>
@@ -2991,7 +3069,7 @@
         <v>2300</v>
       </c>
       <c r="H36" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -3009,13 +3087,13 @@
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -3029,19 +3107,19 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F37">
         <v>29000</v>
@@ -3050,7 +3128,7 @@
         <v>1800</v>
       </c>
       <c r="H37" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3068,13 +3146,13 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q37">
         <v>0</v>
@@ -3088,19 +3166,19 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F38">
         <v>35000</v>
@@ -3109,7 +3187,7 @@
         <v>2400</v>
       </c>
       <c r="H38" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -3127,13 +3205,13 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -3147,19 +3225,19 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F39">
         <v>37000</v>
@@ -3168,7 +3246,7 @@
         <v>2100</v>
       </c>
       <c r="H39" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -3186,13 +3264,13 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q39">
         <v>0</v>
@@ -3206,19 +3284,19 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F40">
         <v>48000</v>
@@ -3227,7 +3305,7 @@
         <v>2400</v>
       </c>
       <c r="H40" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -3245,13 +3323,13 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q40">
         <v>0</v>
@@ -3265,19 +3343,19 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F41">
         <v>35000</v>
@@ -3286,7 +3364,7 @@
         <v>2300</v>
       </c>
       <c r="H41" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -3304,13 +3382,13 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q41">
         <v>0</v>
@@ -3324,19 +3402,19 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F42">
         <v>30000</v>
@@ -3345,7 +3423,7 @@
         <v>2000</v>
       </c>
       <c r="H42" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -3363,13 +3441,13 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q42">
         <v>0</v>
@@ -3383,19 +3461,19 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F43">
         <v>37000</v>
@@ -3404,7 +3482,7 @@
         <v>2400</v>
       </c>
       <c r="H43" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -3422,13 +3500,13 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q43">
         <v>0</v>
@@ -3442,19 +3520,19 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E44" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F44">
         <v>45000</v>
@@ -3463,7 +3541,7 @@
         <v>2200</v>
       </c>
       <c r="H44" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -3481,13 +3559,13 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -3501,19 +3579,19 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E45" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F45">
         <v>31000</v>
@@ -3522,7 +3600,7 @@
         <v>2100</v>
       </c>
       <c r="H45" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -3540,13 +3618,13 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q45">
         <v>0</v>
@@ -3560,19 +3638,19 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F46">
         <v>39000</v>
@@ -3581,7 +3659,7 @@
         <v>2400</v>
       </c>
       <c r="H46" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -3599,13 +3677,13 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q46">
         <v>0</v>
@@ -3614,6 +3692,537 @@
         <v>0</v>
       </c>
       <c r="S46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47">
+        <v>1000</v>
+      </c>
+      <c r="G47">
+        <v>10000</v>
+      </c>
+      <c r="H47" t="s">
+        <v>174</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
+        <v>25</v>
+      </c>
+      <c r="O47" t="s">
+        <v>25</v>
+      </c>
+      <c r="P47" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48">
+        <v>1111</v>
+      </c>
+      <c r="G48">
+        <v>11111</v>
+      </c>
+      <c r="H48" t="s">
+        <v>174</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48" t="s">
+        <v>25</v>
+      </c>
+      <c r="O48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P48" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49">
+        <v>12122</v>
+      </c>
+      <c r="G49">
+        <v>12112</v>
+      </c>
+      <c r="H49" t="s">
+        <v>174</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49" t="s">
+        <v>25</v>
+      </c>
+      <c r="O49" t="s">
+        <v>25</v>
+      </c>
+      <c r="P49" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50">
+        <v>12122</v>
+      </c>
+      <c r="G50">
+        <v>12112</v>
+      </c>
+      <c r="H50" t="s">
+        <v>174</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50" t="s">
+        <v>25</v>
+      </c>
+      <c r="O50" t="s">
+        <v>25</v>
+      </c>
+      <c r="P50" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51">
+        <v>1111</v>
+      </c>
+      <c r="G51">
+        <v>1111</v>
+      </c>
+      <c r="H51" t="s">
+        <v>174</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>25</v>
+      </c>
+      <c r="O51" t="s">
+        <v>25</v>
+      </c>
+      <c r="P51" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" t="s">
+        <v>184</v>
+      </c>
+      <c r="D52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52">
+        <v>1212</v>
+      </c>
+      <c r="G52">
+        <v>1212</v>
+      </c>
+      <c r="H52" t="s">
+        <v>174</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52" t="s">
+        <v>25</v>
+      </c>
+      <c r="O52" t="s">
+        <v>25</v>
+      </c>
+      <c r="P52" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53">
+        <v>100000</v>
+      </c>
+      <c r="G53">
+        <v>200</v>
+      </c>
+      <c r="H53" t="s">
+        <v>187</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53" t="s">
+        <v>25</v>
+      </c>
+      <c r="O53" t="s">
+        <v>25</v>
+      </c>
+      <c r="P53" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54">
+        <v>1000</v>
+      </c>
+      <c r="G54">
+        <v>1000</v>
+      </c>
+      <c r="H54" t="s">
+        <v>191</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
+        <v>25</v>
+      </c>
+      <c r="O54" t="s">
+        <v>25</v>
+      </c>
+      <c r="P54" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" t="s">
+        <v>193</v>
+      </c>
+      <c r="D55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55">
+        <v>1212</v>
+      </c>
+      <c r="G55">
+        <v>1212</v>
+      </c>
+      <c r="H55" t="s">
+        <v>174</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55" t="s">
+        <v>25</v>
+      </c>
+      <c r="O55" t="s">
+        <v>25</v>
+      </c>
+      <c r="P55" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>